<commit_message>
- Colocado o envio de email no endProcess
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robbi9\Documents\UiPath\Teste RPA\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erika\Documents\Uipath\TesteRPA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520FD15E-008F-4DBC-84CD-E4BC0A755920}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2669012-9DA6-4391-B696-BDF53F8B0A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3615" yWindow="1725" windowWidth="16335" windowHeight="11955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -181,6 +181,18 @@
   </si>
   <si>
     <t>sUltimaExecucao</t>
+  </si>
+  <si>
+    <t>sEmail</t>
+  </si>
+  <si>
+    <t>erikalsilva.rpa@gmail.com</t>
+  </si>
+  <si>
+    <t>sPassword</t>
+  </si>
+  <si>
+    <t>acfh coak kqze gyye</t>
   </si>
 </sst>
 </file>
@@ -233,16 +245,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -261,9 +273,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -301,7 +313,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -407,7 +419,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -549,7 +561,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -560,7 +572,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -669,8 +681,22 @@
         <v>44889</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1669,7 +1695,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -2833,7 +2859,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>